<commit_message>
Actualización Solicitud gráfica CN_06_02_CO_REC_40
Actualización Solicitud gráfica CN_06_02_CO_REC_40
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/SolicitudGrafica_CN_06_02_CO_REC40.xlsx
+++ b/fuentes/contenidos/grado06/guion02/SolicitudGrafica_CN_06_02_CO_REC40.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="202">
   <si>
     <t>Fecha:</t>
   </si>
@@ -626,10 +626,13 @@
     <t xml:space="preserve">Cambiar nombres en inglés por:                                                                         nuclear envolope    por      Membrana nuclear                                                  Nucleolus                   por       Nucléolo                                                              Nucleus                       por       Núcleo                                                                                                         endoplasmic reticulum   por   Retículo endoplásmico                                                                  Golgi apparatus      por         Aparato de Golgi                                                                         Cell wall                     por         Pared celular                                                       Cell membrane       por         Membrana celular                                                  Mitochondrion         por        Mitocondria                                                            Cytoplasm                 Por        Citoplasma                                                          Choloplast                 Por       Cloroplasto                                                           Vacuole                     Por        Vacuola            </t>
   </si>
   <si>
-    <t xml:space="preserve">Cambiar nombres en inglés por:                                                                                                                        Nucleolus                   por       Nucléolo                                                              Nucleus                       por       Núcleo                                                                                                         endoplasmic reticulum   por   Retículo endoplásmico                                                                  Golgi apparatus      por         Aparato de Golgi                                                                                                                               Cell membrane       por         Membrana celular                                                  Mitochondrion         por        Mitocondria                                                            Cytoplasm                 Por        Citoplasma                                                         Lysosome                   Por         Lisosoma                                                        Vacuole                     Por        Vacuola               </t>
-  </si>
-  <si>
     <t>CN_06_02_REC40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminar el título de la imagen                                                                                                   Cambiar nombres en inglés por:                                                                                                                        Nucleolus                   por       Nucléolo                                                              Nucleus                       por       Núcleo                                                                                                         endoplasmic reticulum   por   Retículo endoplásmico                                                                  Golgi apparatus      por         Aparato de Golgi                                                                                                                               Cell membrane       por         Membrana celular                                                  Mitochondrion         por        Mitocondria                                                            Cytoplasm                 Por        Citoplasma                                                         Lysosome                   Por         Lisosoma                                                        Vacuole                     Por        Vacuola               </t>
+  </si>
+  <si>
+    <t>Cambiar nombres al español y editar imagen así:</t>
   </si>
 </sst>
 </file>
@@ -1829,6 +1832,61 @@
         <a:xfrm>
           <a:off x="17631833" y="2508249"/>
           <a:ext cx="1907712" cy="1891244"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>35871</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2688772</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1578429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16440150" y="9941871"/>
+          <a:ext cx="2612572" cy="1542558"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2565,9 +2623,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:D2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2766,7 +2824,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>39</v>
@@ -3073,13 +3131,13 @@
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
       </c>
       <c r="B15" s="62">
-        <v>244039624</v>
+        <v>141162034</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3108,9 +3166,11 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="K15" s="66"/>
+        <v>192</v>
+      </c>
+      <c r="K15" s="64" t="s">
+        <v>200</v>
+      </c>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
         <v>F6B</v>
@@ -3159,13 +3219,13 @@
         <v>F7</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="11" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
       <c r="B17" s="62">
-        <v>141162034</v>
+        <v>170485292</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3194,10 +3254,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="K17" s="64" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>

</xml_diff>

<commit_message>
Actualización Sol. Graf. CN 06 02 CO REC 40
Actualización Sol. Graf. CN 06 02 CO REC 40
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/SolicitudGrafica_CN_06_02_CO_REC40.xlsx
+++ b/fuentes/contenidos/grado06/guion02/SolicitudGrafica_CN_06_02_CO_REC40.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_06_02_CO\Recursos realizados por Diego Molina\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="202">
   <si>
     <t>Fecha:</t>
   </si>
@@ -2623,9 +2623,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2973,23 +2973,23 @@
         <v>190</v>
       </c>
       <c r="E11" s="63" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F11" s="13" t="str">
         <f t="shared" ref="F11:F74" ca="1" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_06_02_REC40_IMG02n.jpg</v>
+        <v>CN_06_02_REC40_IMG02.jpg</v>
       </c>
       <c r="G11" s="13" t="str">
         <f ca="1">IF($F11&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>320 x 480 px</v>
+        <v>350 x 230 px</v>
       </c>
       <c r="H11" s="13" t="str">
         <f t="shared" ref="H11:H74" ca="1" si="5">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>CN_06_02_REC40_IMG02a.jpg</v>
+        <v/>
       </c>
       <c r="I11" s="13" t="str">
         <f ca="1">IF(OR($B11&lt;&gt;"",$J11&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 458 px</v>
+        <v/>
       </c>
       <c r="J11" s="64" t="s">
         <v>192</v>
@@ -3102,23 +3102,27 @@
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
       </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="13" t="e">
+      <c r="D14" s="63" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G14" s="13" t="e">
+        <v>CN_06_02_REC40_IMG05n.jpg</v>
+      </c>
+      <c r="G14" s="13" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H14" s="13" t="e">
+        <v>320 x 480 px</v>
+      </c>
+      <c r="H14" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I14" s="13" t="e">
+        <v>CN_06_02_REC40_IMG05a.jpg</v>
+      </c>
+      <c r="I14" s="13" t="str">
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>#N/A</v>
+        <v>800 x 458 px</v>
       </c>
       <c r="J14" s="64" t="s">
         <v>191</v>
@@ -3144,7 +3148,7 @@
         <v>Recurso F6</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E15" s="63" t="s">
         <v>155</v>

</xml_diff>